<commit_message>
EPD Material - addin
</commit_message>
<xml_diff>
--- a/BOM_2.xlsx
+++ b/BOM_2.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="6" documentId="8_{045469B7-985C-4228-A21A-69D8919B4854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8FD6259-E23D-442E-8972-58C168D90E79}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E5275F09-F699-4B09-A0B7-CD6B3C424D26}"/>
+    <workbookView xWindow="28680" yWindow="-1770" windowWidth="29040" windowHeight="15720" xr2:uid="{E5275F09-F699-4B09-A0B7-CD6B3C424D26}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -635,6 +635,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -981,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27E9B65-38E1-444E-ABD2-BFD085016987}">
   <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>